<commit_message>
New CargoSpace for hill climbing algorithm
</commit_message>
<xml_diff>
--- a/Genetic Algorithm Autom Pack/Experiment Data 2.xlsx
+++ b/Genetic Algorithm Autom Pack/Experiment Data 2.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Simon\Documents\GitHub\PP3\Genetic Algorithm Autom Pack\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Desktop\GitHub\PP3\Genetic Algorithm Autom Pack\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -290,7 +290,7 @@
               <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="de-DE"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -492,8 +492,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1806842896"/>
-        <c:axId val="-1806837456"/>
+        <c:axId val="256050136"/>
+        <c:axId val="256078976"/>
       </c:scatterChart>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
@@ -598,11 +598,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2126760208"/>
-        <c:axId val="-2126766736"/>
+        <c:axId val="256525208"/>
+        <c:axId val="256477184"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1806842896"/>
+        <c:axId val="256050136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -674,7 +674,7 @@
                   <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="de-DE"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -712,15 +712,15 @@
                 <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1806837456"/>
+        <c:crossAx val="256078976"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1806837456"/>
+        <c:axId val="256078976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -792,7 +792,7 @@
                   <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="de-DE"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -830,15 +830,15 @@
                 <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1806842896"/>
+        <c:crossAx val="256050136"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2126766736"/>
+        <c:axId val="256477184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -896,7 +896,7 @@
                   <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="de-DE"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -933,15 +933,15 @@
                 <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2126760208"/>
+        <c:crossAx val="256525208"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2126760208"/>
+        <c:axId val="256525208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -951,7 +951,8 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2126766736"/>
+        <c:crossAx val="256477184"/>
+        <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
@@ -990,7 +991,7 @@
               <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="de-DE"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1023,7 +1024,7 @@
           <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
         </a:defRPr>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="de-DE"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1100,7 +1101,7 @@
               <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="de-DE"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1290,8 +1291,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1734144096"/>
-        <c:axId val="-1734144640"/>
+        <c:axId val="256174304"/>
+        <c:axId val="256604440"/>
       </c:scatterChart>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
@@ -1476,11 +1477,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1689109952"/>
-        <c:axId val="-1689106144"/>
+        <c:axId val="256960744"/>
+        <c:axId val="256960360"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1734144096"/>
+        <c:axId val="256174304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1552,7 +1553,7 @@
                   <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="de-DE"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1590,15 +1591,15 @@
                 <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1734144640"/>
+        <c:crossAx val="256604440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1734144640"/>
+        <c:axId val="256604440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1668,7 +1669,7 @@
                   <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="de-DE"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1703,15 +1704,15 @@
                 <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1734144096"/>
+        <c:crossAx val="256174304"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1689106144"/>
+        <c:axId val="256960360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1773,7 +1774,7 @@
                   <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="de-DE"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1808,15 +1809,15 @@
                 <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1689109952"/>
+        <c:crossAx val="256960744"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1689109952"/>
+        <c:axId val="256960744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1826,7 +1827,8 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1689106144"/>
+        <c:crossAx val="256960360"/>
+        <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
@@ -1865,7 +1867,7 @@
               <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="de-DE"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1898,7 +1900,7 @@
           <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
         </a:defRPr>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="de-DE"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1954,7 +1956,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1980,7 +1981,7 @@
               <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="de-DE"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -2256,8 +2257,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1741714432"/>
-        <c:axId val="-1741714976"/>
+        <c:axId val="256574504"/>
+        <c:axId val="256648112"/>
       </c:scatterChart>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
@@ -2528,11 +2529,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1699209808"/>
-        <c:axId val="-1699208720"/>
+        <c:axId val="256662192"/>
+        <c:axId val="256653616"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1741714432"/>
+        <c:axId val="256574504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2578,7 +2579,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2604,7 +2604,7 @@
                   <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="de-DE"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -2642,15 +2642,15 @@
                 <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1741714976"/>
+        <c:crossAx val="256648112"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1741714976"/>
+        <c:axId val="256648112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2697,7 +2697,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2720,7 +2719,7 @@
                   <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="de-DE"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -2755,15 +2754,15 @@
                 <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1741714432"/>
+        <c:crossAx val="256574504"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1699208720"/>
+        <c:axId val="256653616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2812,7 +2811,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2838,7 +2836,7 @@
                   <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="de-DE"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -2873,15 +2871,15 @@
                 <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1699209808"/>
+        <c:crossAx val="256662192"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1699209808"/>
+        <c:axId val="256662192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2891,7 +2889,8 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1699208720"/>
+        <c:crossAx val="256653616"/>
+        <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
@@ -2904,7 +2903,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2930,7 +2928,7 @@
               <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="de-DE"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -2963,7 +2961,7 @@
           <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
         </a:defRPr>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="de-DE"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -3014,7 +3012,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3040,7 +3037,7 @@
               <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="de-DE"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -3316,8 +3313,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1690777392"/>
-        <c:axId val="-1690759984"/>
+        <c:axId val="256251184"/>
+        <c:axId val="256251576"/>
       </c:scatterChart>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
@@ -3588,11 +3585,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2127517488"/>
-        <c:axId val="-1876458368"/>
+        <c:axId val="256252360"/>
+        <c:axId val="256251968"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1690777392"/>
+        <c:axId val="256251184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3643,7 +3640,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -3669,7 +3665,7 @@
                   <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="de-DE"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -3707,15 +3703,15 @@
                 <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1690759984"/>
+        <c:crossAx val="256251576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1690759984"/>
+        <c:axId val="256251576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3762,7 +3758,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -3785,7 +3780,7 @@
                   <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="de-DE"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -3820,15 +3815,15 @@
                 <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1690777392"/>
+        <c:crossAx val="256251184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1876458368"/>
+        <c:axId val="256251968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3864,7 +3859,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -3890,7 +3884,7 @@
                   <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="de-DE"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -3925,15 +3919,15 @@
                 <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2127517488"/>
+        <c:crossAx val="256252360"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2127517488"/>
+        <c:axId val="256252360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3943,7 +3937,8 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1876458368"/>
+        <c:crossAx val="256251968"/>
+        <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
@@ -3956,7 +3951,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3982,7 +3976,7 @@
               <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="de-DE"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -4015,7 +4009,7 @@
           <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
         </a:defRPr>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="de-DE"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -4071,7 +4065,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4097,7 +4090,7 @@
               <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="de-DE"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -4355,8 +4348,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1695787040"/>
-        <c:axId val="-1695788128"/>
+        <c:axId val="256768360"/>
+        <c:axId val="256768752"/>
       </c:scatterChart>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
@@ -4609,11 +4602,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1688694608"/>
-        <c:axId val="-1688695152"/>
+        <c:axId val="256769536"/>
+        <c:axId val="256769144"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1695787040"/>
+        <c:axId val="256768360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4664,7 +4657,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -4690,7 +4682,7 @@
                   <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="de-DE"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -4728,15 +4720,15 @@
                 <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1695788128"/>
+        <c:crossAx val="256768752"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1695788128"/>
+        <c:axId val="256768752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4783,7 +4775,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -4806,7 +4797,7 @@
                   <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="de-DE"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -4841,15 +4832,15 @@
                 <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1695787040"/>
+        <c:crossAx val="256768360"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1688695152"/>
+        <c:axId val="256769144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4886,15 +4877,15 @@
                 <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1688694608"/>
+        <c:crossAx val="256769536"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1688694608"/>
+        <c:axId val="256769536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4904,7 +4895,8 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1688695152"/>
+        <c:crossAx val="256769144"/>
+        <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
@@ -4917,7 +4909,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4943,7 +4934,7 @@
               <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="de-DE"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -4976,7 +4967,7 @@
           <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
         </a:defRPr>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="de-DE"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -5027,7 +5018,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5053,7 +5043,7 @@
               <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="de-DE"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -5347,8 +5337,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2127520208"/>
-        <c:axId val="-1725863904"/>
+        <c:axId val="256770712"/>
+        <c:axId val="256771104"/>
       </c:scatterChart>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
@@ -5637,11 +5627,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2127519120"/>
-        <c:axId val="-1695452816"/>
+        <c:axId val="257143464"/>
+        <c:axId val="257143072"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2127520208"/>
+        <c:axId val="256770712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5687,7 +5677,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -5713,7 +5702,7 @@
                   <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="de-DE"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -5751,15 +5740,15 @@
                 <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1725863904"/>
+        <c:crossAx val="256771104"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1725863904"/>
+        <c:axId val="256771104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5806,7 +5795,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -5829,7 +5817,7 @@
                   <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="de-DE"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -5864,15 +5852,15 @@
                 <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2127520208"/>
+        <c:crossAx val="256770712"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1695452816"/>
+        <c:axId val="257143072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5918,7 +5906,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -5941,7 +5928,7 @@
                   <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="de-DE"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -5976,15 +5963,15 @@
                 <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2127519120"/>
+        <c:crossAx val="257143464"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2127519120"/>
+        <c:axId val="257143464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5994,7 +5981,8 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1695452816"/>
+        <c:crossAx val="257143072"/>
+        <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
@@ -6007,7 +5995,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -6033,7 +6020,7 @@
               <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="de-DE"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -6066,7 +6053,7 @@
           <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
         </a:defRPr>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="de-DE"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -9863,8 +9850,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M187"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="O16" sqref="O16"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10212,7 +10199,7 @@
       <c r="A15" s="3">
         <v>100</v>
       </c>
-      <c r="B15">
+      <c r="B15" s="3">
         <v>240</v>
       </c>
       <c r="C15" s="4">

</xml_diff>

<commit_message>
Small update to the report
</commit_message>
<xml_diff>
--- a/Genetic Algorithm Autom Pack/Experiment Data 2.xlsx
+++ b/Genetic Algorithm Autom Pack/Experiment Data 2.xlsx
@@ -264,7 +264,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -492,8 +491,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="61623376"/>
-        <c:axId val="61622984"/>
+        <c:axId val="255042352"/>
+        <c:axId val="255042744"/>
       </c:scatterChart>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
@@ -598,11 +597,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="61624160"/>
-        <c:axId val="61623768"/>
+        <c:axId val="255043528"/>
+        <c:axId val="255043136"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="61623376"/>
+        <c:axId val="255042352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -648,7 +647,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -715,12 +713,12 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="61622984"/>
+        <c:crossAx val="255042744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="61622984"/>
+        <c:axId val="255042744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -766,7 +764,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -833,12 +830,12 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="61623376"/>
+        <c:crossAx val="255042352"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="61623768"/>
+        <c:axId val="255043136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -870,7 +867,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -936,12 +932,12 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="61624160"/>
+        <c:crossAx val="255043528"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="61624160"/>
+        <c:axId val="255043528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -951,7 +947,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="61623768"/>
+        <c:crossAx val="255043136"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -965,7 +961,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1291,8 +1286,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="61625336"/>
-        <c:axId val="61625728"/>
+        <c:axId val="255044312"/>
+        <c:axId val="255044704"/>
       </c:scatterChart>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
@@ -1477,11 +1472,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="61626512"/>
-        <c:axId val="61626120"/>
+        <c:axId val="255045488"/>
+        <c:axId val="255045096"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="61625336"/>
+        <c:axId val="255044312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1594,12 +1589,12 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="61625728"/>
+        <c:crossAx val="255044704"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="61625728"/>
+        <c:axId val="255044704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1704,12 +1699,12 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="61625336"/>
+        <c:crossAx val="255044312"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="61626120"/>
+        <c:axId val="255045096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1806,12 +1801,12 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="61626512"/>
+        <c:crossAx val="255045488"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="61626512"/>
+        <c:axId val="255045488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1821,7 +1816,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="61626120"/>
+        <c:crossAx val="255045096"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2252,8 +2247,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="61627688"/>
-        <c:axId val="61628080"/>
+        <c:axId val="255702504"/>
+        <c:axId val="255702896"/>
       </c:scatterChart>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
@@ -2524,11 +2519,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="61628864"/>
-        <c:axId val="61628472"/>
+        <c:axId val="255703680"/>
+        <c:axId val="255703288"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="61627688"/>
+        <c:axId val="255702504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2641,12 +2636,12 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="61628080"/>
+        <c:crossAx val="255702896"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="61628080"/>
+        <c:axId val="255702896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2751,12 +2746,12 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="61627688"/>
+        <c:crossAx val="255702504"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="61628472"/>
+        <c:axId val="255703288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2866,12 +2861,12 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="61628864"/>
+        <c:crossAx val="255703680"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="61628864"/>
+        <c:axId val="255703680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2881,7 +2876,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="61628472"/>
+        <c:crossAx val="255703288"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3307,8 +3302,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="242301536"/>
-        <c:axId val="242301928"/>
+        <c:axId val="255704464"/>
+        <c:axId val="255704856"/>
       </c:scatterChart>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
@@ -3579,11 +3574,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="242302712"/>
-        <c:axId val="242302320"/>
+        <c:axId val="255705640"/>
+        <c:axId val="255705248"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="242301536"/>
+        <c:axId val="255704464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3701,12 +3696,12 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="242301928"/>
+        <c:crossAx val="255704856"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="242301928"/>
+        <c:axId val="255704856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3811,12 +3806,12 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="242301536"/>
+        <c:crossAx val="255704464"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="242302320"/>
+        <c:axId val="255705248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3913,12 +3908,12 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="242302712"/>
+        <c:crossAx val="255705640"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="242302712"/>
+        <c:axId val="255705640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3928,7 +3923,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="242302320"/>
+        <c:crossAx val="255705248"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4341,8 +4336,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="242305064"/>
-        <c:axId val="242305456"/>
+        <c:axId val="256064440"/>
+        <c:axId val="256064832"/>
       </c:scatterChart>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
@@ -4595,11 +4590,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="242306240"/>
-        <c:axId val="242305848"/>
+        <c:axId val="256065616"/>
+        <c:axId val="256065224"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="242305064"/>
+        <c:axId val="256064440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4717,12 +4712,12 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="242305456"/>
+        <c:crossAx val="256064832"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="242305456"/>
+        <c:axId val="256064832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4827,12 +4822,12 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="242305064"/>
+        <c:crossAx val="256064440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="242305848"/>
+        <c:axId val="256065224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4869,12 +4864,12 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="242306240"/>
+        <c:crossAx val="256065616"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="242306240"/>
+        <c:axId val="256065616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4884,7 +4879,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="242305848"/>
+        <c:crossAx val="256065224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5328,8 +5323,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="242307416"/>
-        <c:axId val="242307808"/>
+        <c:axId val="256066400"/>
+        <c:axId val="256066792"/>
       </c:scatterChart>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
@@ -5618,11 +5613,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="242308592"/>
-        <c:axId val="242308200"/>
+        <c:axId val="256067576"/>
+        <c:axId val="256067184"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="242307416"/>
+        <c:axId val="256066400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5735,12 +5730,12 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="242307808"/>
+        <c:crossAx val="256066792"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="242307808"/>
+        <c:axId val="256066792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5845,12 +5840,12 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="242307416"/>
+        <c:crossAx val="256066400"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="242308200"/>
+        <c:axId val="256067184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5954,12 +5949,12 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="242308592"/>
+        <c:crossAx val="256067576"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="242308592"/>
+        <c:axId val="256067576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5969,7 +5964,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="242308200"/>
+        <c:crossAx val="256067184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -9839,8 +9834,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M187"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K97" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="P131" sqref="P131"/>
+    <sheetView tabSelected="1" topLeftCell="A61" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F80" sqref="F80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Some more data, updated the report, added some comments in the GA class
</commit_message>
<xml_diff>
--- a/Genetic Algorithm Autom Pack/Experiment Data 2.xlsx
+++ b/Genetic Algorithm Autom Pack/Experiment Data 2.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Desktop\GitHub\PP3\Genetic Algorithm Autom Pack\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Simon\Documents\GitHub\PP3\Genetic Algorithm Autom Pack\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="38">
   <si>
     <t>All experiments run on an i5-4790k 3.5 GHz processor</t>
   </si>
@@ -118,12 +118,36 @@
   <si>
     <t>Tournament size = 10% of population</t>
   </si>
+  <si>
+    <t>% 1D</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>V</t>
+  </si>
+  <si>
+    <t>T (ms)</t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>CrF</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.000"/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -138,6 +162,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -166,7 +196,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -174,11 +204,185 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -195,6 +399,64 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -264,6 +526,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -289,7 +552,7 @@
               <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -491,8 +754,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="255042352"/>
-        <c:axId val="255042744"/>
+        <c:axId val="-674487808"/>
+        <c:axId val="-674486720"/>
       </c:scatterChart>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
@@ -597,11 +860,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="255043528"/>
-        <c:axId val="255043136"/>
+        <c:axId val="-674489440"/>
+        <c:axId val="-674486176"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="255042352"/>
+        <c:axId val="-674487808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -647,6 +910,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -672,7 +936,7 @@
                   <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="de-DE"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -710,15 +974,15 @@
                 <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="255042744"/>
+        <c:crossAx val="-674486720"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="255042744"/>
+        <c:axId val="-674486720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -764,6 +1028,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -789,7 +1054,7 @@
                   <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="de-DE"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -827,15 +1092,15 @@
                 <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="255042352"/>
+        <c:crossAx val="-674487808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="255043136"/>
+        <c:axId val="-674486176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -867,6 +1132,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -892,7 +1158,7 @@
                   <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="de-DE"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -929,15 +1195,15 @@
                 <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="255043528"/>
+        <c:crossAx val="-674489440"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="255043528"/>
+        <c:axId val="-674489440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -947,7 +1213,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="255043136"/>
+        <c:crossAx val="-674486176"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -961,6 +1227,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -986,7 +1253,7 @@
               <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1019,7 +1286,7 @@
           <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
         </a:defRPr>
       </a:pPr>
-      <a:endParaRPr lang="de-DE"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1096,7 +1363,7 @@
               <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1286,8 +1553,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="255044312"/>
-        <c:axId val="255044704"/>
+        <c:axId val="-674485088"/>
+        <c:axId val="-674493792"/>
       </c:scatterChart>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
@@ -1472,11 +1739,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="255045488"/>
-        <c:axId val="255045096"/>
+        <c:axId val="-674482912"/>
+        <c:axId val="-674483456"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="255044312"/>
+        <c:axId val="-674485088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1548,7 +1815,7 @@
                   <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="de-DE"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1586,15 +1853,15 @@
                 <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="255044704"/>
+        <c:crossAx val="-674493792"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="255044704"/>
+        <c:axId val="-674493792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1664,7 +1931,7 @@
                   <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="de-DE"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1696,15 +1963,15 @@
                 <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="255044312"/>
+        <c:crossAx val="-674485088"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="255045096"/>
+        <c:axId val="-674483456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1766,7 +2033,7 @@
                   <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="de-DE"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1798,15 +2065,15 @@
                 <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="255045488"/>
+        <c:crossAx val="-674482912"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="255045488"/>
+        <c:axId val="-674482912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1816,7 +2083,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="255045096"/>
+        <c:crossAx val="-674483456"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1856,7 +2123,7 @@
               <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1889,7 +2156,7 @@
           <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
         </a:defRPr>
       </a:pPr>
-      <a:endParaRPr lang="de-DE"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1971,7 +2238,7 @@
               <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -2247,8 +2514,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="255702504"/>
-        <c:axId val="255702896"/>
+        <c:axId val="-674481824"/>
+        <c:axId val="-674488352"/>
       </c:scatterChart>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
@@ -2519,11 +2786,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="255703680"/>
-        <c:axId val="255703288"/>
+        <c:axId val="-674481280"/>
+        <c:axId val="-674493248"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="255702504"/>
+        <c:axId val="-674481824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2595,7 +2862,7 @@
                   <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="de-DE"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -2633,15 +2900,15 @@
                 <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="255702896"/>
+        <c:crossAx val="-674488352"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="255702896"/>
+        <c:axId val="-674488352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2711,7 +2978,7 @@
                   <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="de-DE"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -2743,15 +3010,15 @@
                 <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="255702504"/>
+        <c:crossAx val="-674481824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="255703288"/>
+        <c:axId val="-674493248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2826,7 +3093,7 @@
                   <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="de-DE"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -2858,15 +3125,15 @@
                 <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="255703680"/>
+        <c:crossAx val="-674481280"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="255703680"/>
+        <c:axId val="-674481280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2876,7 +3143,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="255703288"/>
+        <c:crossAx val="-674493248"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2916,7 +3183,7 @@
               <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -2949,7 +3216,7 @@
           <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
         </a:defRPr>
       </a:pPr>
-      <a:endParaRPr lang="de-DE"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -3026,7 +3293,7 @@
               <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -3302,8 +3569,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="255704464"/>
-        <c:axId val="255704856"/>
+        <c:axId val="-674495968"/>
+        <c:axId val="-674495424"/>
       </c:scatterChart>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
@@ -3574,11 +3841,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="255705640"/>
-        <c:axId val="255705248"/>
+        <c:axId val="-674492704"/>
+        <c:axId val="-674494880"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="255704464"/>
+        <c:axId val="-674495968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3655,7 +3922,7 @@
                   <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="de-DE"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -3693,15 +3960,15 @@
                 <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="255704856"/>
+        <c:crossAx val="-674495424"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="255704856"/>
+        <c:axId val="-674495424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3771,7 +4038,7 @@
                   <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="de-DE"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -3803,15 +4070,15 @@
                 <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="255704464"/>
+        <c:crossAx val="-674495968"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="255705248"/>
+        <c:axId val="-674494880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3873,7 +4140,7 @@
                   <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="de-DE"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -3905,15 +4172,15 @@
                 <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="255705640"/>
+        <c:crossAx val="-674492704"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="255705640"/>
+        <c:axId val="-674492704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3923,7 +4190,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="255705248"/>
+        <c:crossAx val="-674494880"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3963,7 +4230,7 @@
               <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -3996,7 +4263,7 @@
           <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
         </a:defRPr>
       </a:pPr>
-      <a:endParaRPr lang="de-DE"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -4078,7 +4345,7 @@
               <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -4336,8 +4603,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="256064440"/>
-        <c:axId val="256064832"/>
+        <c:axId val="-422918608"/>
+        <c:axId val="-422914800"/>
       </c:scatterChart>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
@@ -4590,11 +4857,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="256065616"/>
-        <c:axId val="256065224"/>
+        <c:axId val="-422915888"/>
+        <c:axId val="-422912080"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="256064440"/>
+        <c:axId val="-422918608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4671,7 +4938,7 @@
                   <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="de-DE"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -4709,15 +4976,15 @@
                 <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="256064832"/>
+        <c:crossAx val="-422914800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="256064832"/>
+        <c:axId val="-422914800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4787,7 +5054,7 @@
                   <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="de-DE"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -4819,15 +5086,15 @@
                 <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="256064440"/>
+        <c:crossAx val="-422918608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="256065224"/>
+        <c:axId val="-422912080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4861,15 +5128,15 @@
                 <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="256065616"/>
+        <c:crossAx val="-422915888"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="256065616"/>
+        <c:axId val="-422915888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4879,7 +5146,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="256065224"/>
+        <c:crossAx val="-422912080"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4919,7 +5186,7 @@
               <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -4952,7 +5219,7 @@
           <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
         </a:defRPr>
       </a:pPr>
-      <a:endParaRPr lang="de-DE"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -5029,7 +5296,7 @@
               <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -5323,8 +5590,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="256066400"/>
-        <c:axId val="256066792"/>
+        <c:axId val="-422920240"/>
+        <c:axId val="-422918064"/>
       </c:scatterChart>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
@@ -5613,11 +5880,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="256067576"/>
-        <c:axId val="256067184"/>
+        <c:axId val="-422925136"/>
+        <c:axId val="-422922960"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="256066400"/>
+        <c:axId val="-422920240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5689,7 +5956,7 @@
                   <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="de-DE"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -5727,15 +5994,15 @@
                 <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="256066792"/>
+        <c:crossAx val="-422918064"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="256066792"/>
+        <c:axId val="-422918064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5805,7 +6072,7 @@
                   <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="de-DE"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -5837,15 +6104,15 @@
                 <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="256066400"/>
+        <c:crossAx val="-422920240"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="256067184"/>
+        <c:axId val="-422922960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5914,7 +6181,7 @@
                   <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="de-DE"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -5946,15 +6213,15 @@
                 <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="256067576"/>
+        <c:crossAx val="-422925136"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="256067576"/>
+        <c:axId val="-422925136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5964,7 +6231,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="256067184"/>
+        <c:crossAx val="-422922960"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6004,7 +6271,7 @@
               <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -6037,7 +6304,7 @@
           <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
         </a:defRPr>
       </a:pPr>
-      <a:endParaRPr lang="de-DE"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -9388,16 +9655,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>750793</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>174811</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>336177</xdr:colOff>
+      <xdr:row>85</xdr:row>
+      <xdr:rowOff>85164</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>672353</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>145676</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>403413</xdr:colOff>
+      <xdr:row>103</xdr:row>
+      <xdr:rowOff>56029</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -9418,16 +9685,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>67234</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>29135</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>123265</xdr:colOff>
+      <xdr:row>105</xdr:row>
+      <xdr:rowOff>6724</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>761999</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>67234</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>537883</xdr:colOff>
+      <xdr:row>122</xdr:row>
+      <xdr:rowOff>44823</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -9448,16 +9715,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>67236</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>62752</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>336178</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>29134</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>24</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>58</xdr:row>
-      <xdr:rowOff>22412</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>504265</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>179294</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -9478,16 +9745,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>33616</xdr:colOff>
-      <xdr:row>58</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>672352</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>85164</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>24</xdr:col>
-      <xdr:colOff>145675</xdr:colOff>
-      <xdr:row>78</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>358587</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>123264</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -9508,16 +9775,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>750795</xdr:colOff>
-      <xdr:row>79</xdr:row>
-      <xdr:rowOff>163607</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>179296</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>107577</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>24</xdr:col>
-      <xdr:colOff>739589</xdr:colOff>
-      <xdr:row>99</xdr:row>
-      <xdr:rowOff>100853</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>504266</xdr:colOff>
+      <xdr:row>83</xdr:row>
+      <xdr:rowOff>44823</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -9538,16 +9805,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>324971</xdr:colOff>
-      <xdr:row>100</xdr:row>
-      <xdr:rowOff>186018</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>235324</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>40342</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>683558</xdr:colOff>
-      <xdr:row>124</xdr:row>
-      <xdr:rowOff>33617</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>168087</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>78441</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -9832,10 +10099,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M187"/>
+  <dimension ref="A1:AA187"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F80" sqref="F80"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="P18" sqref="P18:W24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9852,9 +10119,17 @@
     <col min="10" max="10" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="10" bestFit="1" customWidth="1"/>
     <col min="12" max="13" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="8.5703125" customWidth="1"/>
+    <col min="17" max="17" width="10" customWidth="1"/>
+    <col min="18" max="18" width="12.140625" customWidth="1"/>
+    <col min="19" max="19" width="9.42578125" customWidth="1"/>
+    <col min="20" max="20" width="11.42578125" customWidth="1"/>
+    <col min="21" max="21" width="11.5703125" customWidth="1"/>
+    <col min="22" max="22" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -9862,37 +10137,62 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="P7" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q7" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="R7" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="S7" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="T7" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="U7" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="V7" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="W7" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="Y7" s="3"/>
+    </row>
+    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>6</v>
       </c>
@@ -9932,8 +10232,34 @@
       <c r="M8" s="3" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="P8" s="12">
+        <v>10</v>
+      </c>
+      <c r="Q8" s="13">
+        <v>201.2</v>
+      </c>
+      <c r="R8" s="13">
+        <v>2837.72</v>
+      </c>
+      <c r="S8" s="13">
+        <v>214.76</v>
+      </c>
+      <c r="T8" s="13">
+        <v>34.840000000000003</v>
+      </c>
+      <c r="U8" s="13">
+        <v>10.72</v>
+      </c>
+      <c r="V8" s="13">
+        <v>10.76</v>
+      </c>
+      <c r="W8" s="14">
+        <f>Q8/246</f>
+        <v>0.8178861788617886</v>
+      </c>
+      <c r="Y8" s="4"/>
+    </row>
+    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>10</v>
       </c>
@@ -9973,8 +10299,34 @@
       <c r="M9" s="4">
         <v>10.76</v>
       </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="P9" s="15">
+        <v>20</v>
+      </c>
+      <c r="Q9" s="16">
+        <v>208.08</v>
+      </c>
+      <c r="R9" s="16">
+        <v>7112.32</v>
+      </c>
+      <c r="S9" s="16">
+        <v>180.48</v>
+      </c>
+      <c r="T9" s="16">
+        <v>32.880000000000003</v>
+      </c>
+      <c r="U9" s="16">
+        <v>9.36</v>
+      </c>
+      <c r="V9" s="16">
+        <v>14.4</v>
+      </c>
+      <c r="W9" s="17">
+        <f t="shared" ref="W9:W14" si="0">Q9/246</f>
+        <v>0.84585365853658545</v>
+      </c>
+      <c r="Y9" s="4"/>
+    </row>
+    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>20</v>
       </c>
@@ -10014,8 +10366,34 @@
       <c r="M10" s="4">
         <v>14.4</v>
       </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="P10" s="15">
+        <v>35</v>
+      </c>
+      <c r="Q10" s="16">
+        <v>230.28</v>
+      </c>
+      <c r="R10" s="16">
+        <v>8371.24</v>
+      </c>
+      <c r="S10" s="16">
+        <v>63.52</v>
+      </c>
+      <c r="T10" s="16">
+        <v>35.479999999999997</v>
+      </c>
+      <c r="U10" s="16">
+        <v>8.36</v>
+      </c>
+      <c r="V10" s="16">
+        <v>18.079999999999998</v>
+      </c>
+      <c r="W10" s="17">
+        <f t="shared" si="0"/>
+        <v>0.93609756097560981</v>
+      </c>
+      <c r="Y10" s="4"/>
+    </row>
+    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>35</v>
       </c>
@@ -10055,8 +10433,34 @@
       <c r="M11" s="4">
         <v>18.079999999999998</v>
       </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="P11" s="15">
+        <v>50</v>
+      </c>
+      <c r="Q11" s="16">
+        <v>232.12</v>
+      </c>
+      <c r="R11" s="16">
+        <v>4008.56</v>
+      </c>
+      <c r="S11" s="16">
+        <v>52.72</v>
+      </c>
+      <c r="T11" s="16">
+        <v>34.520000000000003</v>
+      </c>
+      <c r="U11" s="16">
+        <v>8.64</v>
+      </c>
+      <c r="V11" s="16">
+        <v>18.8</v>
+      </c>
+      <c r="W11" s="17">
+        <f t="shared" si="0"/>
+        <v>0.94357723577235775</v>
+      </c>
+      <c r="Y11" s="4"/>
+    </row>
+    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>50</v>
       </c>
@@ -10096,8 +10500,34 @@
       <c r="M12" s="4">
         <v>18.8</v>
       </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="P12" s="15">
+        <v>70</v>
+      </c>
+      <c r="Q12" s="16">
+        <v>234.32</v>
+      </c>
+      <c r="R12" s="16">
+        <v>4652.84</v>
+      </c>
+      <c r="S12" s="16">
+        <v>41.4</v>
+      </c>
+      <c r="T12" s="16">
+        <v>33</v>
+      </c>
+      <c r="U12" s="16">
+        <v>8.2799999999999994</v>
+      </c>
+      <c r="V12" s="16">
+        <v>20.440000000000001</v>
+      </c>
+      <c r="W12" s="17">
+        <f t="shared" si="0"/>
+        <v>0.95252032520325203</v>
+      </c>
+      <c r="Y12" s="4"/>
+    </row>
+    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>70</v>
       </c>
@@ -10137,8 +10567,34 @@
       <c r="M13" s="4">
         <v>20.440000000000001</v>
       </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="P13" s="15">
+        <v>85</v>
+      </c>
+      <c r="Q13" s="16">
+        <v>236.24</v>
+      </c>
+      <c r="R13" s="16">
+        <v>4446.8</v>
+      </c>
+      <c r="S13" s="16">
+        <v>30.68</v>
+      </c>
+      <c r="T13" s="16">
+        <v>32.68</v>
+      </c>
+      <c r="U13" s="16">
+        <v>8.4</v>
+      </c>
+      <c r="V13" s="16">
+        <v>20.92</v>
+      </c>
+      <c r="W13" s="17">
+        <f t="shared" si="0"/>
+        <v>0.96032520325203252</v>
+      </c>
+      <c r="Y13" s="4"/>
+    </row>
+    <row r="14" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="3">
         <v>85</v>
       </c>
@@ -10178,8 +10634,34 @@
       <c r="M14" s="6">
         <v>20.92</v>
       </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="P14" s="18">
+        <v>100</v>
+      </c>
+      <c r="Q14" s="19">
+        <v>236.4</v>
+      </c>
+      <c r="R14" s="19">
+        <v>6531.96</v>
+      </c>
+      <c r="S14" s="19">
+        <v>28.4</v>
+      </c>
+      <c r="T14" s="19">
+        <v>31.84</v>
+      </c>
+      <c r="U14" s="19">
+        <v>8.92</v>
+      </c>
+      <c r="V14" s="19">
+        <v>21.04</v>
+      </c>
+      <c r="W14" s="20">
+        <f t="shared" si="0"/>
+        <v>0.96097560975609764</v>
+      </c>
+      <c r="Y14" s="4"/>
+    </row>
+    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>100</v>
       </c>
@@ -10220,32 +10702,150 @@
         <v>21.04</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="P18" s="25" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q18" s="26" t="s">
+        <v>33</v>
+      </c>
+      <c r="R18" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="S18" s="26" t="s">
+        <v>35</v>
+      </c>
+      <c r="T18" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="U18" s="26" t="s">
+        <v>17</v>
+      </c>
+      <c r="V18" s="26" t="s">
+        <v>18</v>
+      </c>
+      <c r="W18" s="27" t="s">
+        <v>31</v>
+      </c>
+      <c r="X18" s="21"/>
+      <c r="Y18" s="4"/>
+      <c r="Z18" s="21"/>
+      <c r="AA18" s="21"/>
+    </row>
+    <row r="19" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="P19" s="24">
+        <v>0</v>
+      </c>
+      <c r="Q19" s="13">
+        <v>226.84</v>
+      </c>
+      <c r="R19" s="13">
+        <v>31417.759999999998</v>
+      </c>
+      <c r="S19" s="13">
+        <v>78.88</v>
+      </c>
+      <c r="T19" s="13">
+        <v>30.44</v>
+      </c>
+      <c r="U19" s="13">
+        <v>9.2799999999999994</v>
+      </c>
+      <c r="V19" s="13">
+        <v>19.68</v>
+      </c>
+      <c r="W19" s="14">
+        <f>Q19/246</f>
+        <v>0.92211382113821139</v>
+      </c>
+      <c r="X19" s="21"/>
+      <c r="Y19" s="4"/>
+      <c r="Z19" s="21"/>
+      <c r="AA19" s="21"/>
+    </row>
+    <row r="20" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="P20" s="22">
+        <v>1</v>
+      </c>
+      <c r="Q20" s="16">
+        <v>226.2</v>
+      </c>
+      <c r="R20" s="16">
+        <v>31804.6</v>
+      </c>
+      <c r="S20" s="16">
+        <v>83.08</v>
+      </c>
+      <c r="T20" s="16">
+        <v>30.8</v>
+      </c>
+      <c r="U20" s="16">
+        <v>9</v>
+      </c>
+      <c r="V20" s="16">
+        <v>19.559999999999999</v>
+      </c>
+      <c r="W20" s="17">
+        <f t="shared" ref="W20:W24" si="1">Q20/246</f>
+        <v>0.91951219512195115</v>
+      </c>
+      <c r="X20" s="21"/>
+      <c r="Y20" s="4"/>
+      <c r="Z20" s="21"/>
+      <c r="AA20" s="21"/>
+    </row>
+    <row r="21" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O21" t="s">
+        <v>36</v>
+      </c>
+      <c r="P21" s="22">
+        <v>2</v>
+      </c>
+      <c r="Q21" s="16">
+        <v>236.52</v>
+      </c>
+      <c r="R21" s="16">
+        <v>5750.12</v>
+      </c>
+      <c r="S21" s="16">
+        <v>28.92</v>
+      </c>
+      <c r="T21" s="16">
+        <v>32.4</v>
+      </c>
+      <c r="U21" s="16">
+        <v>8.48</v>
+      </c>
+      <c r="V21" s="16">
+        <v>21.08</v>
+      </c>
+      <c r="W21" s="17">
+        <f t="shared" si="1"/>
+        <v>0.96146341463414642</v>
+      </c>
+      <c r="X21" s="21"/>
+      <c r="Y21" s="4"/>
+      <c r="Z21" s="21"/>
+      <c r="AA21" s="21"/>
+    </row>
+    <row r="22" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>19</v>
       </c>
@@ -10285,8 +10885,37 @@
       <c r="M22" s="3" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="P22" s="22">
+        <v>3</v>
+      </c>
+      <c r="Q22" s="16">
+        <v>236.76</v>
+      </c>
+      <c r="R22" s="16">
+        <v>4583.3999999999996</v>
+      </c>
+      <c r="S22" s="16">
+        <v>29.12</v>
+      </c>
+      <c r="T22" s="16">
+        <v>32.68</v>
+      </c>
+      <c r="U22" s="16">
+        <v>7.88</v>
+      </c>
+      <c r="V22" s="16">
+        <v>21.44</v>
+      </c>
+      <c r="W22" s="17">
+        <f t="shared" si="1"/>
+        <v>0.96243902439024387</v>
+      </c>
+      <c r="X22" s="21"/>
+      <c r="Y22" s="4"/>
+      <c r="Z22" s="21"/>
+      <c r="AA22" s="21"/>
+    </row>
+    <row r="23" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
         <v>5</v>
       </c>
@@ -10326,8 +10955,37 @@
       <c r="M23" s="4">
         <v>19.68</v>
       </c>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="P23" s="22">
+        <v>4</v>
+      </c>
+      <c r="Q23" s="16">
+        <v>237.84</v>
+      </c>
+      <c r="R23" s="16">
+        <v>4510.3999999999996</v>
+      </c>
+      <c r="S23" s="16">
+        <v>22.48</v>
+      </c>
+      <c r="T23" s="16">
+        <v>32</v>
+      </c>
+      <c r="U23" s="16">
+        <v>8.16</v>
+      </c>
+      <c r="V23" s="16">
+        <v>21.84</v>
+      </c>
+      <c r="W23" s="17">
+        <f t="shared" si="1"/>
+        <v>0.9668292682926829</v>
+      </c>
+      <c r="X23" s="21"/>
+      <c r="Y23" s="4"/>
+      <c r="Z23" s="21"/>
+      <c r="AA23" s="21"/>
+    </row>
+    <row r="24" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="4">
         <v>10</v>
       </c>
@@ -10367,8 +11025,37 @@
       <c r="M24" s="6">
         <v>20.32</v>
       </c>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="P24" s="23">
+        <v>5</v>
+      </c>
+      <c r="Q24" s="19">
+        <v>237.32</v>
+      </c>
+      <c r="R24" s="19">
+        <v>4475.2</v>
+      </c>
+      <c r="S24" s="19">
+        <v>25.64</v>
+      </c>
+      <c r="T24" s="19">
+        <v>32.32</v>
+      </c>
+      <c r="U24" s="19">
+        <v>8.0399999999999991</v>
+      </c>
+      <c r="V24" s="19">
+        <v>21.64</v>
+      </c>
+      <c r="W24" s="20">
+        <f t="shared" si="1"/>
+        <v>0.96471544715447155</v>
+      </c>
+      <c r="X24" s="21"/>
+      <c r="Y24" s="4"/>
+      <c r="Z24" s="21"/>
+      <c r="AA24" s="21"/>
+    </row>
+    <row r="25" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
         <v>15</v>
       </c>
@@ -10409,7 +11096,7 @@
         <v>20.6</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
         <v>20</v>
       </c>
@@ -10450,7 +11137,7 @@
         <v>20.16</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A27" s="3">
         <v>30</v>
       </c>
@@ -10491,7 +11178,7 @@
         <v>19.28</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A28" s="3">
         <v>40</v>
       </c>
@@ -10532,17 +11219,17 @@
         <v>19.239999999999998</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>3</v>
       </c>
@@ -14274,6 +14961,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Latest update to report
</commit_message>
<xml_diff>
--- a/Genetic Algorithm Autom Pack/Experiment Data 2.xlsx
+++ b/Genetic Algorithm Autom Pack/Experiment Data 2.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Simon\Documents\GitHub\PP3\Genetic Algorithm Autom Pack\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Desktop\GitHub\PP3\Genetic Algorithm Autom Pack\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="55">
   <si>
     <t>All experiments run on an i5-4790k 3.5 GHz processor</t>
   </si>
@@ -138,6 +138,57 @@
   </si>
   <si>
     <t>CrF</t>
+  </si>
+  <si>
+    <t>Test No.</t>
+  </si>
+  <si>
+    <t>12479.16</t>
+  </si>
+  <si>
+    <t>61883.96</t>
+  </si>
+  <si>
+    <t>45626.04</t>
+  </si>
+  <si>
+    <t>715.68</t>
+  </si>
+  <si>
+    <t>85670.68</t>
+  </si>
+  <si>
+    <t>29.72</t>
+  </si>
+  <si>
+    <t>81555.08</t>
+  </si>
+  <si>
+    <t>121.44</t>
+  </si>
+  <si>
+    <t>45034.76</t>
+  </si>
+  <si>
+    <t>81.12</t>
+  </si>
+  <si>
+    <t>Small</t>
+  </si>
+  <si>
+    <t>Big</t>
+  </si>
+  <si>
+    <t>Compact</t>
+  </si>
+  <si>
+    <t>Long</t>
+  </si>
+  <si>
+    <t>Flat</t>
+  </si>
+  <si>
+    <t>plus D</t>
   </si>
 </sst>
 </file>
@@ -382,7 +433,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -459,6 +510,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -526,7 +583,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -552,7 +608,7 @@
               <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="de-DE"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -754,8 +810,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-674487808"/>
-        <c:axId val="-674486720"/>
+        <c:axId val="264703056"/>
+        <c:axId val="264703440"/>
       </c:scatterChart>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
@@ -860,11 +916,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-674489440"/>
-        <c:axId val="-674486176"/>
+        <c:axId val="264704208"/>
+        <c:axId val="264703824"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-674487808"/>
+        <c:axId val="264703056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -910,7 +966,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -936,7 +991,7 @@
                   <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="de-DE"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -974,15 +1029,15 @@
                 <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-674486720"/>
+        <c:crossAx val="264703440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-674486720"/>
+        <c:axId val="264703440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1028,7 +1083,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1054,7 +1108,7 @@
                   <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="de-DE"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1092,15 +1146,15 @@
                 <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-674487808"/>
+        <c:crossAx val="264703056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-674486176"/>
+        <c:axId val="264703824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1132,7 +1186,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1158,7 +1211,7 @@
                   <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="de-DE"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1195,15 +1248,15 @@
                 <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-674489440"/>
+        <c:crossAx val="264704208"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-674489440"/>
+        <c:axId val="264704208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1213,7 +1266,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-674486176"/>
+        <c:crossAx val="264703824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1227,7 +1280,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1253,7 +1305,7 @@
               <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="de-DE"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1286,7 +1338,7 @@
           <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
         </a:defRPr>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="de-DE"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1337,7 +1389,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1363,7 +1414,7 @@
               <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="de-DE"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1553,8 +1604,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-674485088"/>
-        <c:axId val="-674493792"/>
+        <c:axId val="264453104"/>
+        <c:axId val="264476016"/>
       </c:scatterChart>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
@@ -1739,11 +1790,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-674482912"/>
-        <c:axId val="-674483456"/>
+        <c:axId val="264491120"/>
+        <c:axId val="264484592"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-674485088"/>
+        <c:axId val="264453104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1789,7 +1840,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1815,7 +1865,7 @@
                   <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="de-DE"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1853,15 +1903,15 @@
                 <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-674493792"/>
+        <c:crossAx val="264476016"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-674493792"/>
+        <c:axId val="264476016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1908,7 +1958,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1931,7 +1980,7 @@
                   <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="de-DE"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1963,15 +2012,15 @@
                 <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-674485088"/>
+        <c:crossAx val="264453104"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-674483456"/>
+        <c:axId val="264484592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2007,7 +2056,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2033,7 +2081,7 @@
                   <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="de-DE"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -2065,15 +2113,15 @@
                 <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-674482912"/>
+        <c:crossAx val="264491120"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-674482912"/>
+        <c:axId val="264491120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2083,7 +2131,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-674483456"/>
+        <c:crossAx val="264484592"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2097,7 +2145,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2123,7 +2170,7 @@
               <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="de-DE"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -2156,7 +2203,7 @@
           <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
         </a:defRPr>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="de-DE"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -2238,7 +2285,7 @@
               <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="de-DE"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -2514,8 +2561,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-674481824"/>
-        <c:axId val="-674488352"/>
+        <c:axId val="264559400"/>
+        <c:axId val="264572072"/>
       </c:scatterChart>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
@@ -2786,11 +2833,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-674481280"/>
-        <c:axId val="-674493248"/>
+        <c:axId val="264585128"/>
+        <c:axId val="264584744"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-674481824"/>
+        <c:axId val="264559400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2862,7 +2909,7 @@
                   <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="de-DE"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -2900,15 +2947,15 @@
                 <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-674488352"/>
+        <c:crossAx val="264572072"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-674488352"/>
+        <c:axId val="264572072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2978,7 +3025,7 @@
                   <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="de-DE"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -3010,15 +3057,15 @@
                 <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-674481824"/>
+        <c:crossAx val="264559400"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-674493248"/>
+        <c:axId val="264584744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3093,7 +3140,7 @@
                   <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="de-DE"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -3125,15 +3172,15 @@
                 <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-674481280"/>
+        <c:crossAx val="264585128"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-674481280"/>
+        <c:axId val="264585128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3143,7 +3190,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-674493248"/>
+        <c:crossAx val="264584744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3183,7 +3230,7 @@
               <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="de-DE"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -3216,7 +3263,7 @@
           <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
         </a:defRPr>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="de-DE"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -3267,7 +3314,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3293,7 +3339,7 @@
               <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="de-DE"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -3569,8 +3615,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-674495968"/>
-        <c:axId val="-674495424"/>
+        <c:axId val="264604376"/>
+        <c:axId val="264920936"/>
       </c:scatterChart>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
@@ -3841,11 +3887,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-674492704"/>
-        <c:axId val="-674494880"/>
+        <c:axId val="264921720"/>
+        <c:axId val="264921328"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-674495968"/>
+        <c:axId val="264604376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3896,7 +3942,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -3922,7 +3967,7 @@
                   <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="de-DE"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -3960,15 +4005,15 @@
                 <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-674495424"/>
+        <c:crossAx val="264920936"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-674495424"/>
+        <c:axId val="264920936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4015,7 +4060,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -4038,7 +4082,7 @@
                   <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="de-DE"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -4070,15 +4114,15 @@
                 <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-674495968"/>
+        <c:crossAx val="264604376"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-674494880"/>
+        <c:axId val="264921328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4114,7 +4158,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -4140,7 +4183,7 @@
                   <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="de-DE"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -4172,15 +4215,15 @@
                 <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-674492704"/>
+        <c:crossAx val="264921720"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-674492704"/>
+        <c:axId val="264921720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4190,7 +4233,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-674494880"/>
+        <c:crossAx val="264921328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4204,7 +4247,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4230,7 +4272,7 @@
               <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="de-DE"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -4263,7 +4305,7 @@
           <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
         </a:defRPr>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="de-DE"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -4319,7 +4361,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4345,7 +4386,7 @@
               <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="de-DE"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -4603,8 +4644,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-422918608"/>
-        <c:axId val="-422914800"/>
+        <c:axId val="264922504"/>
+        <c:axId val="264922896"/>
       </c:scatterChart>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
@@ -4857,11 +4898,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-422915888"/>
-        <c:axId val="-422912080"/>
+        <c:axId val="264923680"/>
+        <c:axId val="264923288"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-422918608"/>
+        <c:axId val="264922504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4912,7 +4953,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -4938,7 +4978,7 @@
                   <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="de-DE"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -4976,15 +5016,15 @@
                 <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-422914800"/>
+        <c:crossAx val="264922896"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-422914800"/>
+        <c:axId val="264922896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5031,7 +5071,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -5054,7 +5093,7 @@
                   <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="de-DE"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -5086,15 +5125,15 @@
                 <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-422918608"/>
+        <c:crossAx val="264922504"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-422912080"/>
+        <c:axId val="264923288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5128,15 +5167,15 @@
                 <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-422915888"/>
+        <c:crossAx val="264923680"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-422915888"/>
+        <c:axId val="264923680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5146,7 +5185,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-422912080"/>
+        <c:crossAx val="264923288"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5160,7 +5199,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5186,7 +5224,7 @@
               <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="de-DE"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -5219,7 +5257,7 @@
           <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
         </a:defRPr>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="de-DE"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -5296,7 +5334,7 @@
               <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="de-DE"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -5590,8 +5628,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-422920240"/>
-        <c:axId val="-422918064"/>
+        <c:axId val="264924464"/>
+        <c:axId val="265121120"/>
       </c:scatterChart>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
@@ -5880,11 +5918,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-422925136"/>
-        <c:axId val="-422922960"/>
+        <c:axId val="265121904"/>
+        <c:axId val="265121512"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-422920240"/>
+        <c:axId val="264924464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5956,7 +5994,7 @@
                   <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="de-DE"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -5994,15 +6032,15 @@
                 <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-422918064"/>
+        <c:crossAx val="265121120"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-422918064"/>
+        <c:axId val="265121120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6072,7 +6110,7 @@
                   <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="de-DE"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -6104,15 +6142,15 @@
                 <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-422920240"/>
+        <c:crossAx val="264924464"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-422922960"/>
+        <c:axId val="265121512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6181,7 +6219,7 @@
                   <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="de-DE"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -6213,15 +6251,15 @@
                 <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-422925136"/>
+        <c:crossAx val="265121904"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-422925136"/>
+        <c:axId val="265121904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6231,7 +6269,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-422922960"/>
+        <c:crossAx val="265121512"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6271,7 +6309,7 @@
               <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="de-DE"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -6304,7 +6342,7 @@
           <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
         </a:defRPr>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="de-DE"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -10099,10 +10137,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AA187"/>
+  <dimension ref="A1:AC187"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="P18" sqref="P18:W24"/>
+    <sheetView tabSelected="1" topLeftCell="U1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AB17" sqref="AB17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10129,7 +10167,7 @@
     <col min="23" max="23" width="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -10137,32 +10175,32 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -10190,9 +10228,23 @@
       <c r="W7" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="Y7" s="3"/>
-    </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y7" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="Z7" s="28" t="s">
+        <v>33</v>
+      </c>
+      <c r="AA7" s="28" t="s">
+        <v>34</v>
+      </c>
+      <c r="AB7" s="28" t="s">
+        <v>35</v>
+      </c>
+      <c r="AC7" s="28" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>6</v>
       </c>
@@ -10257,9 +10309,27 @@
         <f>Q8/246</f>
         <v>0.8178861788617886</v>
       </c>
-      <c r="Y8" s="4"/>
-    </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="X8" t="s">
+        <v>49</v>
+      </c>
+      <c r="Y8" s="4">
+        <v>1</v>
+      </c>
+      <c r="Z8" s="3">
+        <v>289.26</v>
+      </c>
+      <c r="AA8" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="AB8" s="3">
+        <v>50</v>
+      </c>
+      <c r="AC8" s="29">
+        <f>Z8/330</f>
+        <v>0.87654545454545452</v>
+      </c>
+    </row>
+    <row r="9" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>10</v>
       </c>
@@ -10324,9 +10394,27 @@
         <f t="shared" ref="W9:W14" si="0">Q9/246</f>
         <v>0.84585365853658545</v>
       </c>
-      <c r="Y9" s="4"/>
-    </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="X9" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y9" s="4">
+        <v>2</v>
+      </c>
+      <c r="Z9" s="3">
+        <v>10</v>
+      </c>
+      <c r="AA9" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="AB9" s="3">
+        <v>123</v>
+      </c>
+      <c r="AC9" s="29">
+        <f>Z9/11</f>
+        <v>0.90909090909090906</v>
+      </c>
+    </row>
+    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>20</v>
       </c>
@@ -10391,9 +10479,27 @@
         <f t="shared" si="0"/>
         <v>0.93609756097560981</v>
       </c>
-      <c r="Y10" s="4"/>
-    </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="X10" t="s">
+        <v>51</v>
+      </c>
+      <c r="Y10" s="4">
+        <v>3</v>
+      </c>
+      <c r="Z10" s="3">
+        <v>108.56</v>
+      </c>
+      <c r="AA10" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="AB10" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="AC10" s="29">
+        <f>Z10/165</f>
+        <v>0.65793939393939394</v>
+      </c>
+    </row>
+    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>35</v>
       </c>
@@ -10458,9 +10564,27 @@
         <f t="shared" si="0"/>
         <v>0.94357723577235775</v>
       </c>
-      <c r="Y11" s="4"/>
-    </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="X11" t="s">
+        <v>52</v>
+      </c>
+      <c r="Y11" s="4">
+        <v>4</v>
+      </c>
+      <c r="Z11" s="3">
+        <v>248.6</v>
+      </c>
+      <c r="AA11" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="AB11" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="AC11" s="29">
+        <f>Z11/264</f>
+        <v>0.94166666666666665</v>
+      </c>
+    </row>
+    <row r="12" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>50</v>
       </c>
@@ -10525,9 +10649,27 @@
         <f t="shared" si="0"/>
         <v>0.95252032520325203</v>
       </c>
-      <c r="Y12" s="4"/>
-    </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="X12" t="s">
+        <v>53</v>
+      </c>
+      <c r="Y12" s="4">
+        <v>5</v>
+      </c>
+      <c r="Z12" s="3">
+        <v>130.68</v>
+      </c>
+      <c r="AA12" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="AB12" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="AC12" s="29">
+        <f>Z12/146</f>
+        <v>0.89506849315068493</v>
+      </c>
+    </row>
+    <row r="13" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>70</v>
       </c>
@@ -10592,9 +10734,27 @@
         <f t="shared" si="0"/>
         <v>0.96032520325203252</v>
       </c>
-      <c r="Y13" s="4"/>
-    </row>
-    <row r="14" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="X13" t="s">
+        <v>54</v>
+      </c>
+      <c r="Y13" s="4">
+        <v>6</v>
+      </c>
+      <c r="Z13" s="3">
+        <v>219</v>
+      </c>
+      <c r="AA13" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="AB13" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="AC13" s="3">
+        <f>Z13/230</f>
+        <v>0.95217391304347831</v>
+      </c>
+    </row>
+    <row r="14" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="3">
         <v>85</v>
       </c>
@@ -10660,8 +10820,12 @@
         <v>0.96097560975609764</v>
       </c>
       <c r="Y14" s="4"/>
-    </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z14" s="3"/>
+      <c r="AA14" s="3"/>
+      <c r="AB14" s="3"/>
+      <c r="AC14" s="3"/>
+    </row>
+    <row r="15" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>100</v>
       </c>

</xml_diff>

<commit_message>
Some more report stuff
</commit_message>
<xml_diff>
--- a/Genetic Algorithm Autom Pack/Experiment Data 2.xlsx
+++ b/Genetic Algorithm Autom Pack/Experiment Data 2.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="50">
   <si>
     <t>All experiments run on an i5-4790k 3.5 GHz processor</t>
   </si>
@@ -163,6 +163,18 @@
   <si>
     <t>plus D, E</t>
   </si>
+  <si>
+    <t>plus D, E, F</t>
+  </si>
+  <si>
+    <t>15 of each</t>
+  </si>
+  <si>
+    <t>10 of each</t>
+  </si>
+  <si>
+    <t>infinite</t>
+  </si>
 </sst>
 </file>
 
@@ -220,7 +232,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -402,11 +414,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -490,6 +511,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -786,8 +811,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1960109424"/>
-        <c:axId val="1960103440"/>
+        <c:axId val="1934546912"/>
+        <c:axId val="1934550176"/>
       </c:scatterChart>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
@@ -892,11 +917,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1960097456"/>
-        <c:axId val="1960109968"/>
+        <c:axId val="1934550720"/>
+        <c:axId val="1934547456"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1960109424"/>
+        <c:axId val="1934546912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1008,12 +1033,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1960103440"/>
+        <c:crossAx val="1934550176"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1960103440"/>
+        <c:axId val="1934550176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1125,12 +1150,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1960109424"/>
+        <c:crossAx val="1934546912"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1960109968"/>
+        <c:axId val="1934547456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1227,12 +1252,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1960097456"/>
+        <c:crossAx val="1934550720"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1960097456"/>
+        <c:axId val="1934550720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1242,7 +1267,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1960109968"/>
+        <c:crossAx val="1934547456"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1580,8 +1605,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1960098000"/>
-        <c:axId val="1960104528"/>
+        <c:axId val="1934542560"/>
+        <c:axId val="1934543648"/>
       </c:scatterChart>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
@@ -1766,11 +1791,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1773945248"/>
-        <c:axId val="1960110512"/>
+        <c:axId val="1934543104"/>
+        <c:axId val="1934535488"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1960098000"/>
+        <c:axId val="1934542560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1882,12 +1907,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1960104528"/>
+        <c:crossAx val="1934543648"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1960104528"/>
+        <c:axId val="1934543648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1991,12 +2016,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1960098000"/>
+        <c:crossAx val="1934542560"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1960110512"/>
+        <c:axId val="1934535488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2092,12 +2117,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1773945248"/>
+        <c:crossAx val="1934543104"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1773945248"/>
+        <c:axId val="1934543104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2107,7 +2132,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1960110512"/>
+        <c:crossAx val="1934535488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2536,8 +2561,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1773944160"/>
-        <c:axId val="1773946336"/>
+        <c:axId val="1934537120"/>
+        <c:axId val="1934537664"/>
       </c:scatterChart>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
@@ -2808,11 +2833,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1934541472"/>
-        <c:axId val="1773947424"/>
+        <c:axId val="1934538752"/>
+        <c:axId val="1934538208"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1773944160"/>
+        <c:axId val="1934537120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2924,12 +2949,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1773946336"/>
+        <c:crossAx val="1934537664"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1773946336"/>
+        <c:axId val="1934537664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3033,12 +3058,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1773944160"/>
+        <c:crossAx val="1934537120"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1773947424"/>
+        <c:axId val="1934538208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3147,12 +3172,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1934541472"/>
+        <c:crossAx val="1934538752"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1934541472"/>
+        <c:axId val="1934538752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3162,7 +3187,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1773947424"/>
+        <c:crossAx val="1934538208"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3586,8 +3611,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1934550176"/>
-        <c:axId val="1934550720"/>
+        <c:axId val="1960101808"/>
+        <c:axId val="1960097456"/>
       </c:scatterChart>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
@@ -3858,11 +3883,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1676004896"/>
-        <c:axId val="1934536032"/>
+        <c:axId val="1960102896"/>
+        <c:axId val="1960110512"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1934550176"/>
+        <c:axId val="1960101808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3979,12 +4004,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1934550720"/>
+        <c:crossAx val="1960097456"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1934550720"/>
+        <c:axId val="1960097456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4088,12 +4113,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1934550176"/>
+        <c:crossAx val="1960101808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1934536032"/>
+        <c:axId val="1960110512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4189,12 +4214,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1676004896"/>
+        <c:crossAx val="1960102896"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1676004896"/>
+        <c:axId val="1960102896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4204,7 +4229,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1934536032"/>
+        <c:crossAx val="1960110512"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4615,8 +4640,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2056885344"/>
-        <c:axId val="2056882624"/>
+        <c:axId val="1960107248"/>
+        <c:axId val="1960103440"/>
       </c:scatterChart>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
@@ -4869,11 +4894,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2056879360"/>
-        <c:axId val="2056883168"/>
+        <c:axId val="1960108880"/>
+        <c:axId val="1960100176"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2056885344"/>
+        <c:axId val="1960107248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4990,12 +5015,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2056882624"/>
+        <c:crossAx val="1960103440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2056882624"/>
+        <c:axId val="1960103440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5099,12 +5124,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2056885344"/>
+        <c:crossAx val="1960107248"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2056883168"/>
+        <c:axId val="1960100176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5141,12 +5166,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2056879360"/>
+        <c:crossAx val="1960108880"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2056879360"/>
+        <c:axId val="1960108880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5156,7 +5181,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2056883168"/>
+        <c:crossAx val="1960100176"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5598,8 +5623,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2056876096"/>
-        <c:axId val="2056881536"/>
+        <c:axId val="1960109424"/>
+        <c:axId val="1960109968"/>
       </c:scatterChart>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
@@ -5888,11 +5913,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2056878816"/>
-        <c:axId val="2056888608"/>
+        <c:axId val="1677058160"/>
+        <c:axId val="1960111600"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2056876096"/>
+        <c:axId val="1960109424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6004,12 +6029,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2056881536"/>
+        <c:crossAx val="1960109968"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2056881536"/>
+        <c:axId val="1960109968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6113,12 +6138,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2056876096"/>
+        <c:crossAx val="1960109424"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2056888608"/>
+        <c:axId val="1960111600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6221,12 +6246,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2056878816"/>
+        <c:crossAx val="1677058160"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2056878816"/>
+        <c:axId val="1677058160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6236,7 +6261,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2056888608"/>
+        <c:crossAx val="1960111600"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -10103,10 +10128,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AC187"/>
+  <dimension ref="A1:AD187"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="O1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AC13" sqref="AC13"/>
+      <selection activeCell="AF8" sqref="AF8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10133,7 +10158,7 @@
     <col min="23" max="23" width="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -10141,32 +10166,32 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -10210,7 +10235,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>6</v>
       </c>
@@ -10295,7 +10320,7 @@
         <v>0.87654545454545452</v>
       </c>
     </row>
-    <row r="9" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>10</v>
       </c>
@@ -10380,7 +10405,7 @@
         <v>0.90909090909090906</v>
       </c>
     </row>
-    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>20</v>
       </c>
@@ -10465,7 +10490,7 @@
         <v>0.65793939393939394</v>
       </c>
     </row>
-    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>35</v>
       </c>
@@ -10550,7 +10575,7 @@
         <v>0.94166666666666665</v>
       </c>
     </row>
-    <row r="12" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>50</v>
       </c>
@@ -10635,7 +10660,7 @@
         <v>0.89506849315068493</v>
       </c>
     </row>
-    <row r="13" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>70</v>
       </c>
@@ -10707,20 +10732,23 @@
         <v>6</v>
       </c>
       <c r="Z13" s="3">
-        <v>185.28</v>
+        <v>186.24</v>
       </c>
       <c r="AA13" s="30">
-        <v>5555.32</v>
+        <v>33130.76</v>
       </c>
       <c r="AB13" s="30">
-        <v>99</v>
+        <v>165.52</v>
       </c>
       <c r="AC13" s="29">
         <f>Z13/195</f>
-        <v>0.95015384615384613</v>
-      </c>
-    </row>
-    <row r="14" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>0.95507692307692316</v>
+      </c>
+      <c r="AD13" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="14" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="3">
         <v>85</v>
       </c>
@@ -10804,8 +10832,11 @@
         <f>Z14/198</f>
         <v>0.94747474747474747</v>
       </c>
-    </row>
-    <row r="15" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AD14" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="15" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>100</v>
       </c>
@@ -10845,13 +10876,81 @@
       <c r="M15" s="4">
         <v>21.04</v>
       </c>
-    </row>
-    <row r="17" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="X15" t="s">
+        <v>46</v>
+      </c>
+      <c r="Y15" s="4">
+        <v>8</v>
+      </c>
+      <c r="Z15" s="3">
+        <v>140.04</v>
+      </c>
+      <c r="AA15" s="3">
+        <v>37154.92</v>
+      </c>
+      <c r="AB15" s="3">
+        <v>220.4</v>
+      </c>
+      <c r="AC15" s="29">
+        <f>Z15/148</f>
+        <v>0.94621621621621621</v>
+      </c>
+      <c r="AD15" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="16" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="X16" t="s">
+        <v>44</v>
+      </c>
+      <c r="Y16" s="3">
+        <v>9</v>
+      </c>
+      <c r="Z16" s="3">
+        <v>213.36</v>
+      </c>
+      <c r="AA16" s="3">
+        <v>51289.88</v>
+      </c>
+      <c r="AB16" s="3">
+        <v>80.2</v>
+      </c>
+      <c r="AC16" s="29">
+        <f>Z16/247</f>
+        <v>0.86380566801619441</v>
+      </c>
+      <c r="AD16" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="17" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="18" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="X17" t="s">
+        <v>45</v>
+      </c>
+      <c r="Y17" s="4">
+        <v>10</v>
+      </c>
+      <c r="Z17" s="4">
+        <v>201.36</v>
+      </c>
+      <c r="AA17" s="4">
+        <v>72838.039999999994</v>
+      </c>
+      <c r="AB17" s="3">
+        <v>66.56</v>
+      </c>
+      <c r="AC17" s="29">
+        <f>Z17/247</f>
+        <v>0.81522267206477739</v>
+      </c>
+      <c r="AD17" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="18" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>24</v>
       </c>
@@ -10879,12 +10978,30 @@
       <c r="W18" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="X18" s="21"/>
-      <c r="Y18" s="4"/>
-      <c r="Z18" s="21"/>
-      <c r="AA18" s="21"/>
-    </row>
-    <row r="19" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="X18" s="32" t="s">
+        <v>46</v>
+      </c>
+      <c r="Y18" s="4">
+        <v>11</v>
+      </c>
+      <c r="Z18" s="3">
+        <v>204.12</v>
+      </c>
+      <c r="AA18" s="3">
+        <v>73388.08</v>
+      </c>
+      <c r="AB18" s="3">
+        <v>74.239999999999995</v>
+      </c>
+      <c r="AC18" s="29">
+        <f>Z18/247</f>
+        <v>0.82639676113360327</v>
+      </c>
+      <c r="AD18" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="19" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>3</v>
       </c>
@@ -10915,10 +11032,12 @@
       </c>
       <c r="X19" s="21"/>
       <c r="Y19" s="4"/>
-      <c r="Z19" s="21"/>
-      <c r="AA19" s="21"/>
-    </row>
-    <row r="20" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="Z19" s="4"/>
+      <c r="AA19" s="4"/>
+      <c r="AB19" s="3"/>
+      <c r="AC19" s="29"/>
+    </row>
+    <row r="20" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>4</v>
       </c>
@@ -10951,8 +11070,9 @@
       <c r="Y20" s="4"/>
       <c r="Z20" s="21"/>
       <c r="AA20" s="21"/>
-    </row>
-    <row r="21" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AC20" s="31"/>
+    </row>
+    <row r="21" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>5</v>
       </c>
@@ -10988,8 +11108,9 @@
       <c r="Y21" s="4"/>
       <c r="Z21" s="21"/>
       <c r="AA21" s="21"/>
-    </row>
-    <row r="22" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AC21" s="31"/>
+    </row>
+    <row r="22" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>19</v>
       </c>
@@ -11058,8 +11179,9 @@
       <c r="Y22" s="4"/>
       <c r="Z22" s="21"/>
       <c r="AA22" s="21"/>
-    </row>
-    <row r="23" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AC22" s="31"/>
+    </row>
+    <row r="23" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
         <v>5</v>
       </c>
@@ -11128,8 +11250,9 @@
       <c r="Y23" s="4"/>
       <c r="Z23" s="21"/>
       <c r="AA23" s="21"/>
-    </row>
-    <row r="24" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AC23" s="31"/>
+    </row>
+    <row r="24" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="4">
         <v>10</v>
       </c>
@@ -11198,8 +11321,9 @@
       <c r="Y24" s="4"/>
       <c r="Z24" s="21"/>
       <c r="AA24" s="21"/>
-    </row>
-    <row r="25" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AC24" s="31"/>
+    </row>
+    <row r="25" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
         <v>15</v>
       </c>
@@ -11239,8 +11363,9 @@
       <c r="M25" s="4">
         <v>20.6</v>
       </c>
-    </row>
-    <row r="26" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AC25" s="31"/>
+    </row>
+    <row r="26" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
         <v>20</v>
       </c>
@@ -11281,7 +11406,7 @@
         <v>20.16</v>
       </c>
     </row>
-    <row r="27" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A27" s="3">
         <v>30</v>
       </c>
@@ -11322,7 +11447,7 @@
         <v>19.28</v>
       </c>
     </row>
-    <row r="28" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A28" s="3">
         <v>40</v>
       </c>
@@ -11363,17 +11488,17 @@
         <v>19.239999999999998</v>
       </c>
     </row>
-    <row r="30" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="32" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>3</v>
       </c>

</xml_diff>